<commit_message>
Computed all Baseline Results
</commit_message>
<xml_diff>
--- a/Results/All Training Results.xlsx
+++ b/Results/All Training Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96b2e28e11ffcb6a/Dokumente/Studium-Vincents-Surface/Master/Unterlagen/Master Thesis/Repository/MasterThesis/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{E9FDFF15-62A2-4FB9-B4E9-0CC2653326D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6A210A1-4D87-4F5D-8AF2-4A9D69FC36BE}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="13_ncr:1_{E9FDFF15-62A2-4FB9-B4E9-0CC2653326D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD0D7F44-47EA-4EDB-8EA9-1DEB16BD4200}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="33">
   <si>
     <t>Inputs</t>
   </si>
@@ -103,6 +103,30 @@
   </si>
   <si>
     <t>Legend</t>
+  </si>
+  <si>
+    <t>Bukhsh et al</t>
+  </si>
+  <si>
+    <t>next activity</t>
+  </si>
+  <si>
+    <t>remaining time</t>
+  </si>
+  <si>
+    <t>next time</t>
+  </si>
+  <si>
+    <t>no prefix weightning</t>
+  </si>
+  <si>
+    <t>with prefix weightning</t>
+  </si>
+  <si>
+    <t>#####</t>
+  </si>
+  <si>
+    <t>Wang et al</t>
   </si>
 </sst>
 </file>
@@ -273,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -359,19 +383,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -420,8 +431,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -703,11 +736,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB34"/>
+  <dimension ref="A1:AB44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA16" sqref="AA16"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,36 +774,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="35" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37"/>
-      <c r="H1" s="35" t="s">
+      <c r="E1" s="58"/>
+      <c r="F1" s="59"/>
+      <c r="H1" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
       <c r="Z1" s="1" t="s">
         <v>19</v>
       </c>
@@ -799,36 +832,36 @@
       <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="35" t="s">
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="36"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="35" t="s">
+      <c r="L2" s="58"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="35" t="s">
+      <c r="O2" s="58"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="36"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="35" t="s">
+      <c r="R2" s="58"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="36"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="35" t="s">
+      <c r="U2" s="58"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="37"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="59"/>
     </row>
     <row r="3" spans="1:28" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
@@ -925,7 +958,7 @@
       <c r="M4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="44">
+      <c r="N4" s="39">
         <v>0.44190000000000002</v>
       </c>
       <c r="O4" s="13" t="s">
@@ -964,10 +997,10 @@
       <c r="Z4">
         <v>1</v>
       </c>
-      <c r="AA4" s="53" t="s">
+      <c r="AA4" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="AB4" s="54" t="s">
+      <c r="AB4" s="49" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1038,7 +1071,7 @@
       <c r="Z5">
         <v>1</v>
       </c>
-      <c r="AA5" s="55" t="s">
+      <c r="AA5" s="50" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1055,7 +1088,7 @@
       <c r="G6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="44">
+      <c r="H6" s="39">
         <v>0.85350000000000004</v>
       </c>
       <c r="I6" s="13" t="s">
@@ -1064,7 +1097,7 @@
       <c r="J6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="44">
+      <c r="K6" s="39">
         <v>0.74839999999999995</v>
       </c>
       <c r="L6" s="13" t="s">
@@ -1082,7 +1115,7 @@
       <c r="P6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="40">
+      <c r="Q6" s="35">
         <v>0.81830000000000003</v>
       </c>
       <c r="R6" s="13" t="s">
@@ -1091,7 +1124,7 @@
       <c r="S6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="44">
+      <c r="T6" s="39">
         <v>0.81850000000000001</v>
       </c>
       <c r="U6" s="13" t="s">
@@ -1100,7 +1133,7 @@
       <c r="V6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="W6" s="40">
+      <c r="W6" s="35">
         <v>0.63290000000000002</v>
       </c>
       <c r="X6" s="13" t="s">
@@ -1127,7 +1160,7 @@
       <c r="G7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="41">
+      <c r="H7" s="36">
         <v>0.84389999999999998</v>
       </c>
       <c r="I7" s="13" t="s">
@@ -1136,7 +1169,7 @@
       <c r="J7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="41">
+      <c r="K7" s="36">
         <v>0.73919999999999997</v>
       </c>
       <c r="L7" s="13" t="s">
@@ -1154,7 +1187,7 @@
       <c r="P7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="45">
+      <c r="Q7" s="40">
         <v>0.89039999999999997</v>
       </c>
       <c r="R7" s="13" t="s">
@@ -1466,7 +1499,7 @@
       <c r="V11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="W11" s="46">
+      <c r="W11" s="41">
         <v>0.6512</v>
       </c>
       <c r="X11" s="17" t="s">
@@ -1506,7 +1539,7 @@
       <c r="K12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="39">
+      <c r="L12" s="34">
         <v>1.0375000000000001</v>
       </c>
       <c r="M12" s="15" t="s">
@@ -1542,7 +1575,7 @@
       <c r="W12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="X12" s="39">
+      <c r="X12" s="34">
         <v>2.1368</v>
       </c>
       <c r="Y12" s="15" t="s">
@@ -1566,7 +1599,7 @@
       <c r="H13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="47">
+      <c r="I13" s="42">
         <v>0.34520000000000001</v>
       </c>
       <c r="J13" s="15" t="s">
@@ -1575,7 +1608,7 @@
       <c r="K13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="47">
+      <c r="L13" s="42">
         <v>0.88759999999999994</v>
       </c>
       <c r="M13" s="15" t="s">
@@ -1593,7 +1626,7 @@
       <c r="Q13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R13" s="47">
+      <c r="R13" s="42">
         <v>4.3693999999999997</v>
       </c>
       <c r="S13" s="15" t="s">
@@ -1638,7 +1671,7 @@
       <c r="H14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="34">
         <v>0.35410000000000003</v>
       </c>
       <c r="J14" s="15" t="s">
@@ -1656,7 +1689,7 @@
       <c r="N14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O14" s="50">
+      <c r="O14" s="45">
         <v>2.1171000000000002</v>
       </c>
       <c r="P14" s="15" t="s">
@@ -1746,7 +1779,7 @@
       <c r="T15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U15" s="42">
+      <c r="U15" s="37">
         <v>6.1245000000000003</v>
       </c>
       <c r="V15" s="15" t="s">
@@ -1878,7 +1911,7 @@
       <c r="N17" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="O17" s="52">
+      <c r="O17" s="47">
         <v>2.3104</v>
       </c>
       <c r="P17" s="18" t="s">
@@ -2014,7 +2047,7 @@
       <c r="L19" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M19" s="49">
+      <c r="M19" s="44">
         <v>4.8825000000000003</v>
       </c>
       <c r="N19" s="3" t="s">
@@ -2340,7 +2373,7 @@
       <c r="U23" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="V23" s="51">
+      <c r="V23" s="46">
         <v>5.4713000000000003</v>
       </c>
       <c r="W23" s="16" t="s">
@@ -2349,7 +2382,7 @@
       <c r="X23" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="Y23" s="51">
+      <c r="Y23" s="46">
         <v>17.053799999999999</v>
       </c>
       <c r="Z23" s="28">
@@ -2485,7 +2518,7 @@
       <c r="S25" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="T25" s="45">
+      <c r="T25" s="40">
         <v>0.7147</v>
       </c>
       <c r="U25" s="13">
@@ -2497,7 +2530,7 @@
       <c r="W25" s="3">
         <v>0.63280000000000003</v>
       </c>
-      <c r="X25" s="47">
+      <c r="X25" s="42">
         <v>1.0860000000000001</v>
       </c>
       <c r="Y25" s="15" t="s">
@@ -2557,7 +2590,7 @@
       <c r="R26" s="13">
         <v>18.3842</v>
       </c>
-      <c r="S26" s="38">
+      <c r="S26" s="33">
         <v>18.3842</v>
       </c>
       <c r="T26" s="3" t="s">
@@ -2707,7 +2740,7 @@
       <c r="Q28" s="3">
         <v>0.81559999999999999</v>
       </c>
-      <c r="R28" s="39">
+      <c r="R28" s="34">
         <v>6.8630000000000004</v>
       </c>
       <c r="S28" s="15">
@@ -2728,7 +2761,7 @@
       <c r="X28" s="13">
         <v>2.391</v>
       </c>
-      <c r="Y28" s="38">
+      <c r="Y28" s="33">
         <v>36.1111</v>
       </c>
       <c r="Z28" s="28">
@@ -2761,7 +2794,7 @@
       <c r="I29" s="13">
         <v>0.35680000000000001</v>
       </c>
-      <c r="J29" s="43">
+      <c r="J29" s="38">
         <v>4.4371999999999998</v>
       </c>
       <c r="K29" s="3">
@@ -2788,7 +2821,7 @@
       <c r="R29" s="13">
         <v>4.7807000000000004</v>
       </c>
-      <c r="S29" s="49">
+      <c r="S29" s="44">
         <v>12.882</v>
       </c>
       <c r="T29" s="3">
@@ -2872,7 +2905,7 @@
       <c r="T30" s="3">
         <v>0.81420000000000003</v>
       </c>
-      <c r="U30" s="50">
+      <c r="U30" s="45">
         <v>4.9617000000000004</v>
       </c>
       <c r="V30" s="15" t="s">
@@ -2929,7 +2962,7 @@
       <c r="M31" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="N31" s="45">
+      <c r="N31" s="40">
         <v>0.1368</v>
       </c>
       <c r="O31" s="13">
@@ -2998,7 +3031,7 @@
       <c r="I32" s="13">
         <v>0.40510000000000002</v>
       </c>
-      <c r="J32" s="48">
+      <c r="J32" s="43">
         <v>4.2904999999999998</v>
       </c>
       <c r="K32" s="3">
@@ -3007,7 +3040,7 @@
       <c r="L32" s="13">
         <v>1.1151</v>
       </c>
-      <c r="M32" s="38">
+      <c r="M32" s="33">
         <v>5.1002000000000001</v>
       </c>
       <c r="N32" s="3">
@@ -3016,7 +3049,7 @@
       <c r="O32" s="13">
         <v>2.3732000000000002</v>
       </c>
-      <c r="P32" s="38">
+      <c r="P32" s="33">
         <v>24.7624</v>
       </c>
       <c r="Q32" s="3">
@@ -3034,7 +3067,7 @@
       <c r="U32" s="13">
         <v>4.9919000000000002</v>
       </c>
-      <c r="V32" s="38">
+      <c r="V32" s="33">
         <v>6.6573000000000002</v>
       </c>
       <c r="W32" s="3">
@@ -3061,70 +3094,70 @@
       <c r="C33" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="34" t="s">
+      <c r="D33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="16">
+      <c r="H33" s="3">
         <v>0.81599999999999995</v>
       </c>
-      <c r="I33" s="17">
+      <c r="I33" s="13">
         <v>0.38140000000000002</v>
       </c>
-      <c r="J33" s="18">
+      <c r="J33" s="15">
         <v>4.5377999999999998</v>
       </c>
-      <c r="K33" s="16">
+      <c r="K33" s="3">
         <v>0.7117</v>
       </c>
-      <c r="L33" s="17">
+      <c r="L33" s="13">
         <v>1.2461</v>
       </c>
-      <c r="M33" s="18">
+      <c r="M33" s="15">
         <v>6.0350999999999999</v>
       </c>
-      <c r="N33" s="16">
+      <c r="N33" s="3">
         <v>0.12540000000000001</v>
       </c>
-      <c r="O33" s="17">
+      <c r="O33" s="13">
         <v>2.5150000000000001</v>
       </c>
-      <c r="P33" s="51">
+      <c r="P33" s="44">
         <v>24.1693</v>
       </c>
-      <c r="Q33" s="16">
+      <c r="Q33" s="3">
         <v>0.88880000000000003</v>
       </c>
-      <c r="R33" s="17">
+      <c r="R33" s="13">
         <v>4.4576000000000002</v>
       </c>
-      <c r="S33" s="18">
+      <c r="S33" s="15">
         <v>13.1434</v>
       </c>
-      <c r="T33" s="16">
+      <c r="T33" s="3">
         <v>0.68500000000000005</v>
       </c>
-      <c r="U33" s="17">
+      <c r="U33" s="13">
         <v>6.2248999999999999</v>
       </c>
-      <c r="V33" s="18">
+      <c r="V33" s="15">
         <v>5.5426000000000002</v>
       </c>
-      <c r="W33" s="16">
+      <c r="W33" s="3">
         <v>0.624</v>
       </c>
-      <c r="X33" s="17">
+      <c r="X33" s="13">
         <v>1.4293</v>
       </c>
-      <c r="Y33" s="18">
+      <c r="Y33" s="15">
         <v>17.058199999999999</v>
       </c>
       <c r="Z33" s="28">
@@ -3132,10 +3165,670 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="52"/>
+      <c r="C34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K34" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="N34" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="O34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="P34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q34" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="S34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="T34" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="U34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="V34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="W34" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="X34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z34" s="51"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A35" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="54"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="54"/>
+      <c r="H35" s="3">
+        <v>0.85340000000000005</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K35" s="3">
+        <v>0.70779999999999998</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M35" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N35" s="3">
+        <v>0.32540000000000002</v>
+      </c>
+      <c r="O35" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="P35" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>0.93540000000000001</v>
+      </c>
+      <c r="R35" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="S35" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="T35" s="3">
+        <v>0.85880000000000001</v>
+      </c>
+      <c r="U35" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="V35" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="W35" s="3">
+        <v>0.48830000000000001</v>
+      </c>
+      <c r="X35" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y35" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A36" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="54"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="54"/>
+      <c r="H36" s="3">
+        <v>0.84360000000000002</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J36" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="3">
+        <v>0.67490000000000006</v>
+      </c>
+      <c r="L36" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M36" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N36" s="3">
+        <v>0.44969999999999999</v>
+      </c>
+      <c r="O36" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="P36" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>0.89029999999999998</v>
+      </c>
+      <c r="R36" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="S36" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="T36" s="3">
+        <v>0.80359999999999998</v>
+      </c>
+      <c r="U36" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="V36" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="W36" s="3">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="X36" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y36" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A37" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="54"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="54"/>
+      <c r="H37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" s="13">
+        <v>0.23150000000000001</v>
+      </c>
+      <c r="J37" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L37" s="13">
+        <v>0.88439999999999996</v>
+      </c>
+      <c r="M37" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O37" s="13">
+        <v>2.2128000000000001</v>
+      </c>
+      <c r="P37" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R37" s="13">
+        <v>3.3368000000000002</v>
+      </c>
+      <c r="S37" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="T37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U37" s="13">
+        <v>2.9287999999999998</v>
+      </c>
+      <c r="V37" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="W37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="X37" s="13">
+        <v>1.4496</v>
+      </c>
+      <c r="Y37" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A38" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="54"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" s="54"/>
+      <c r="H38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I38" s="13">
+        <v>0.29430000000000001</v>
+      </c>
+      <c r="J38" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L38" s="13">
+        <v>0.80869999999999997</v>
+      </c>
+      <c r="M38" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O38" s="13">
+        <v>2.0485000000000002</v>
+      </c>
+      <c r="P38" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R38" s="13">
+        <v>4.3906999999999998</v>
+      </c>
+      <c r="S38" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="T38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U38" s="13">
+        <v>4.1426999999999996</v>
+      </c>
+      <c r="V38" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="W38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="X38" s="13">
+        <v>1.9936</v>
+      </c>
+      <c r="Y38" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A39" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="54"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="54"/>
+      <c r="H39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J39" s="15">
+        <v>4.8632</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L39" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M39" s="15">
+        <v>7.0350000000000001</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O39" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="P39" s="15">
+        <v>33.589799999999997</v>
+      </c>
+      <c r="Q39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R39" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="S39" s="15">
+        <v>10.5786</v>
+      </c>
+      <c r="T39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U39" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="V39" s="15">
+        <v>3.5762999999999998</v>
+      </c>
+      <c r="W39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="X39" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y39" s="15">
+        <v>51.069400000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A40" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="54"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="54"/>
+      <c r="H40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40" s="15">
+        <v>6.2042999999999999</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L40" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M40" s="15">
+        <v>5.6321000000000003</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O40" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="P40" s="15">
+        <v>42.519500000000001</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R40" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="S40" s="15">
+        <v>15.641299999999999</v>
+      </c>
+      <c r="T40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U40" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="V40" s="15">
+        <v>5.2355</v>
+      </c>
+      <c r="W40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="X40" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y40" s="15">
+        <v>31.696999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="52"/>
+      <c r="C42" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H42" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="J42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K42" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="N42" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="O42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="P42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q42" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="S42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="T42" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="U42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="V42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="W42" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="X42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y42" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="D43" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" s="54"/>
+      <c r="H43" s="3">
+        <v>0.85980000000000001</v>
+      </c>
+      <c r="I43" s="13">
+        <v>0.2387</v>
+      </c>
+      <c r="J43" s="15">
+        <v>4.0755999999999997</v>
+      </c>
+      <c r="K43" s="3">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="L43" s="13">
+        <v>0.95430000000000004</v>
+      </c>
+      <c r="M43" s="15">
+        <v>7.5523999999999996</v>
+      </c>
+      <c r="N43" s="3">
+        <v>0.28270000000000001</v>
+      </c>
+      <c r="O43" s="13">
+        <v>2.4620000000000002</v>
+      </c>
+      <c r="P43" s="15">
+        <v>32.567999999999998</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>0.94540000000000002</v>
+      </c>
+      <c r="R43" s="13">
+        <v>3.0952000000000002</v>
+      </c>
+      <c r="S43" s="15">
+        <v>8.8493999999999993</v>
+      </c>
+      <c r="T43" s="3">
+        <v>0.88380000000000003</v>
+      </c>
+      <c r="U43" s="13">
+        <v>2.8222999999999998</v>
+      </c>
+      <c r="V43" s="15">
+        <v>3.4337</v>
+      </c>
+      <c r="W43" s="3">
+        <v>0.49430000000000002</v>
+      </c>
+      <c r="X43" s="13">
+        <v>1.3720000000000001</v>
+      </c>
+      <c r="Y43" s="15">
+        <v>43.605200000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="D44" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="54"/>
+      <c r="H44" s="3">
+        <v>0.85240000000000005</v>
+      </c>
+      <c r="I44" s="13">
+        <v>0.29620000000000002</v>
+      </c>
+      <c r="J44" s="15">
+        <v>5.9962</v>
+      </c>
+      <c r="K44" s="3">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="L44" s="13">
+        <v>0.7329</v>
+      </c>
+      <c r="M44" s="15">
+        <v>6.4417</v>
+      </c>
+      <c r="N44" s="3">
+        <v>0.40960000000000002</v>
+      </c>
+      <c r="O44" s="13">
+        <v>2.3052000000000001</v>
+      </c>
+      <c r="P44" s="15">
+        <v>38.090400000000002</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>0.89690000000000003</v>
+      </c>
+      <c r="R44" s="13">
+        <v>4.3170000000000002</v>
+      </c>
+      <c r="S44" s="15">
+        <v>14.4948</v>
+      </c>
+      <c r="T44" s="3">
+        <v>0.84309999999999996</v>
+      </c>
+      <c r="U44" s="13">
+        <v>4.1882000000000001</v>
+      </c>
+      <c r="V44" s="15">
+        <v>5.1932999999999998</v>
+      </c>
+      <c r="W44" s="3">
+        <v>0.63970000000000005</v>
+      </c>
+      <c r="X44" s="13">
+        <v>1.6580999999999999</v>
+      </c>
+      <c r="Y44" s="15">
+        <v>30.416899999999998</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="AA3:AB3"/>
+  <mergeCells count="26">
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
@@ -3145,6 +3838,23 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:P2"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>